<commit_message>
This is my Chartbuilder homework
Health care exchanges data
</commit_message>
<xml_diff>
--- a/Assignments/ChartBuilder/Exercise1/Chartbuilder1.xlsx
+++ b/Assignments/ChartBuilder/Exercise1/Chartbuilder1.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30000" yWindow="280" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="-30000" yWindow="285" windowWidth="21720" windowHeight="13620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Qualified Plans v Average" sheetId="2" r:id="rId2"/>
+    <sheet name="Male and Female" sheetId="3" r:id="rId3"/>
+    <sheet name="States' Plans" sheetId="4" r:id="rId4"/>
+    <sheet name="Bronze v Catastrophic" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="56">
   <si>
     <t>State</t>
   </si>
@@ -158,16 +161,47 @@
   </si>
   <si>
     <t>AverageLowestBronzeTaxCredit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Males With health insurance coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Males   No health insurance coverage</t>
+  </si>
+  <si>
+    <t>Females With health insurance coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Females No health insurance coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Males 25 to 34 years:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Females 25 to 34 years:</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Average Bronze</t>
+  </si>
+  <si>
+    <t>Bronze Average</t>
+  </si>
+  <si>
+    <t>Catastrophic average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -198,13 +232,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="SansSerif"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,7 +268,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,16 +324,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="56">
+    <cellStyle name="Comma" xfId="55" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -664,23 +727,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1890,202 +1955,426 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>106</v>
+      </c>
+      <c r="C5" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>102</v>
+      </c>
+      <c r="C7" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>58</v>
+      </c>
+      <c r="C11" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43</v>
+      </c>
+      <c r="C16" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>40</v>
+      </c>
+      <c r="C22" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>52</v>
+      </c>
+      <c r="C25" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>46</v>
+      </c>
+      <c r="C26" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>53</v>
+      </c>
+      <c r="C27" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>56</v>
+      </c>
+      <c r="C28" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>26</v>
+      </c>
+      <c r="C29" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>32</v>
+      </c>
+      <c r="C30" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>59</v>
+      </c>
+      <c r="C31" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>54</v>
+      </c>
+      <c r="C32" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>82</v>
+      </c>
+      <c r="C33" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>47</v>
+      </c>
+      <c r="C34" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>97</v>
+      </c>
+      <c r="C35" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>12</v>
+      </c>
+      <c r="C36" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>16</v>
+      </c>
+      <c r="C37" s="4">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2096,4 +2385,2078 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5">
+        <v>2009</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2010</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E1" s="5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20013400</v>
+      </c>
+      <c r="C2" s="7">
+        <v>19551177</v>
+      </c>
+      <c r="D2" s="7">
+        <v>19885213</v>
+      </c>
+      <c r="E2" s="7">
+        <v>20195255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6">
+        <v>13588853</v>
+      </c>
+      <c r="C3" s="7">
+        <v>13087851</v>
+      </c>
+      <c r="D3" s="7">
+        <v>13466003</v>
+      </c>
+      <c r="E3" s="7">
+        <v>13829297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="8">
+        <v>6424547</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6463326</v>
+      </c>
+      <c r="D4" s="7">
+        <v>6419210</v>
+      </c>
+      <c r="E4" s="7">
+        <v>6365958</v>
+      </c>
+      <c r="F4">
+        <f>SUM(B4:E4)</f>
+        <v>25673041</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6">
+        <v>20143686</v>
+      </c>
+      <c r="C5" s="7">
+        <v>20277773</v>
+      </c>
+      <c r="D5" s="7">
+        <v>20524743</v>
+      </c>
+      <c r="E5" s="7">
+        <v>20758075</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6">
+        <v>15617535</v>
+      </c>
+      <c r="C6" s="7">
+        <v>15534035</v>
+      </c>
+      <c r="D6" s="7">
+        <v>15718481</v>
+      </c>
+      <c r="E6" s="7">
+        <v>15957882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4526151</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4743738</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4806262</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4800193</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7" si="0">SUM(B7:E7)</f>
+        <v>18876344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2009</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2010</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="8">
+        <v>6424547</v>
+      </c>
+      <c r="C13" s="7">
+        <v>6463326</v>
+      </c>
+      <c r="D13" s="7">
+        <v>6419210</v>
+      </c>
+      <c r="E13" s="7">
+        <v>6365958</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="6">
+        <v>4526151</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4743738</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4806262</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4800193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="8">
+        <v>6424547</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4526151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>2010</v>
+      </c>
+      <c r="B18" s="7">
+        <v>6463326</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4743738</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>2011</v>
+      </c>
+      <c r="B19" s="7">
+        <v>6419210</v>
+      </c>
+      <c r="C19" s="7">
+        <v>4806262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>2012</v>
+      </c>
+      <c r="B20" s="7">
+        <v>6365958</v>
+      </c>
+      <c r="C20" s="7">
+        <v>4800193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <v>254</v>
+      </c>
+      <c r="C2" s="2">
+        <v>312</v>
+      </c>
+      <c r="D2" s="2">
+        <v>401</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2">
+        <v>254</v>
+      </c>
+      <c r="H2" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>162</v>
+      </c>
+      <c r="C3" s="2">
+        <v>200</v>
+      </c>
+      <c r="D3" s="2">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>162</v>
+      </c>
+      <c r="H3" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>181</v>
+      </c>
+      <c r="C4" s="2">
+        <v>231</v>
+      </c>
+      <c r="D4" s="2">
+        <v>263</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>181</v>
+      </c>
+      <c r="H4" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>141</v>
+      </c>
+      <c r="C5" s="2">
+        <v>164</v>
+      </c>
+      <c r="D5" s="2">
+        <v>187</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>141</v>
+      </c>
+      <c r="H5" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>203</v>
+      </c>
+      <c r="C6" s="2">
+        <v>234</v>
+      </c>
+      <c r="D6" s="2">
+        <v>282</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>203</v>
+      </c>
+      <c r="H6" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>169</v>
+      </c>
+      <c r="C7" s="2">
+        <v>200</v>
+      </c>
+      <c r="D7" s="2">
+        <v>229</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>169</v>
+      </c>
+      <c r="H7" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>179</v>
+      </c>
+      <c r="C8" s="2">
+        <v>208</v>
+      </c>
+      <c r="D8" s="2">
+        <v>242</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2">
+        <v>179</v>
+      </c>
+      <c r="H8" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>139</v>
+      </c>
+      <c r="C9" s="2">
+        <v>175</v>
+      </c>
+      <c r="D9" s="2">
+        <v>203</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2">
+        <v>139</v>
+      </c>
+      <c r="H9" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>150</v>
+      </c>
+      <c r="C10" s="2">
+        <v>182</v>
+      </c>
+      <c r="D10" s="2">
+        <v>211</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2">
+        <v>150</v>
+      </c>
+      <c r="H10" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>134</v>
+      </c>
+      <c r="C11" s="2">
+        <v>180</v>
+      </c>
+      <c r="D11" s="2">
+        <v>210</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <v>134</v>
+      </c>
+      <c r="H11" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>200</v>
+      </c>
+      <c r="C12" s="2">
+        <v>258</v>
+      </c>
+      <c r="D12" s="2">
+        <v>332</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2">
+        <v>200</v>
+      </c>
+      <c r="H12" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>130</v>
+      </c>
+      <c r="C13" s="2">
+        <v>171</v>
+      </c>
+      <c r="D13" s="2">
+        <v>192</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2">
+        <v>130</v>
+      </c>
+      <c r="H13" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>175</v>
+      </c>
+      <c r="C14" s="2">
+        <v>235</v>
+      </c>
+      <c r="D14" s="2">
+        <v>253</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2">
+        <v>175</v>
+      </c>
+      <c r="H14" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>216</v>
+      </c>
+      <c r="C15" s="2">
+        <v>255</v>
+      </c>
+      <c r="D15" s="2">
+        <v>336</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2">
+        <v>216</v>
+      </c>
+      <c r="H15" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>146</v>
+      </c>
+      <c r="C16" s="2">
+        <v>178</v>
+      </c>
+      <c r="D16" s="2">
+        <v>218</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2">
+        <v>146</v>
+      </c>
+      <c r="H16" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>162</v>
+      </c>
+      <c r="C17" s="2">
+        <v>211</v>
+      </c>
+      <c r="D17" s="2">
+        <v>242</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2">
+        <v>162</v>
+      </c>
+      <c r="H17" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>225</v>
+      </c>
+      <c r="C18" s="2">
+        <v>265</v>
+      </c>
+      <c r="D18" s="2">
+        <v>321</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="2">
+        <v>225</v>
+      </c>
+      <c r="H18" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>165</v>
+      </c>
+      <c r="C19" s="2">
+        <v>204</v>
+      </c>
+      <c r="D19" s="2">
+        <v>222</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2">
+        <v>165</v>
+      </c>
+      <c r="H19" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>186</v>
+      </c>
+      <c r="C20" s="2">
+        <v>237</v>
+      </c>
+      <c r="D20" s="2">
+        <v>283</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="2">
+        <v>186</v>
+      </c>
+      <c r="H20" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>185</v>
+      </c>
+      <c r="C21" s="2">
+        <v>230</v>
+      </c>
+      <c r="D21" s="2">
+        <v>259</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="2">
+        <v>185</v>
+      </c>
+      <c r="H21" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>159</v>
+      </c>
+      <c r="C22" s="2">
+        <v>196</v>
+      </c>
+      <c r="D22" s="2">
+        <v>232</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="2">
+        <v>159</v>
+      </c>
+      <c r="H22" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>186</v>
+      </c>
+      <c r="C23" s="2">
+        <v>236</v>
+      </c>
+      <c r="D23" s="2">
+        <v>281</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="2">
+        <v>186</v>
+      </c>
+      <c r="H23" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>219</v>
+      </c>
+      <c r="C24" s="2">
+        <v>253</v>
+      </c>
+      <c r="D24" s="2">
+        <v>303</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="2">
+        <v>219</v>
+      </c>
+      <c r="H24" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>143</v>
+      </c>
+      <c r="C25" s="2">
+        <v>181</v>
+      </c>
+      <c r="D25" s="2">
+        <v>204</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="2">
+        <v>143</v>
+      </c>
+      <c r="H25" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>177</v>
+      </c>
+      <c r="C26" s="2">
+        <v>200</v>
+      </c>
+      <c r="D26" s="2">
+        <v>243</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="2">
+        <v>177</v>
+      </c>
+      <c r="H26" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>114</v>
+      </c>
+      <c r="C27" s="2">
+        <v>169</v>
+      </c>
+      <c r="D27" s="2">
+        <v>203</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="2">
+        <v>114</v>
+      </c>
+      <c r="H27" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>151</v>
+      </c>
+      <c r="C28" s="2">
+        <v>170</v>
+      </c>
+      <c r="D28" s="2">
+        <v>205</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="2">
+        <v>151</v>
+      </c>
+      <c r="H28" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>176</v>
+      </c>
+      <c r="C29" s="2">
+        <v>219</v>
+      </c>
+      <c r="D29" s="2">
+        <v>259</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="2">
+        <v>176</v>
+      </c>
+      <c r="H29" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>196</v>
+      </c>
+      <c r="C30" s="2">
+        <v>225</v>
+      </c>
+      <c r="D30" s="2">
+        <v>272</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="2">
+        <v>196</v>
+      </c>
+      <c r="H30" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>119</v>
+      </c>
+      <c r="C31" s="2">
+        <v>155</v>
+      </c>
+      <c r="D31" s="2">
+        <v>205</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="2">
+        <v>119</v>
+      </c>
+      <c r="H31" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>139</v>
+      </c>
+      <c r="C32" s="2">
+        <v>189</v>
+      </c>
+      <c r="D32" s="2">
+        <v>225</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="2">
+        <v>139</v>
+      </c>
+      <c r="H32" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>153</v>
+      </c>
+      <c r="C33" s="2">
+        <v>183</v>
+      </c>
+      <c r="D33" s="2">
+        <v>212</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="2">
+        <v>153</v>
+      </c>
+      <c r="H33" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>156</v>
+      </c>
+      <c r="C34" s="2">
+        <v>213</v>
+      </c>
+      <c r="D34" s="2">
+        <v>253</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="2">
+        <v>156</v>
+      </c>
+      <c r="H34" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>189</v>
+      </c>
+      <c r="C35" s="2">
+        <v>227</v>
+      </c>
+      <c r="D35" s="2">
+        <v>280</v>
+      </c>
+      <c r="F35" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="2">
+        <v>189</v>
+      </c>
+      <c r="H35" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>185</v>
+      </c>
+      <c r="C36" s="2">
+        <v>218</v>
+      </c>
+      <c r="D36" s="2">
+        <v>266</v>
+      </c>
+      <c r="F36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" s="2">
+        <v>185</v>
+      </c>
+      <c r="H36" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>286</v>
+      </c>
+      <c r="C37" s="2">
+        <v>324</v>
+      </c>
+      <c r="D37" s="2">
+        <v>365</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="2">
+        <v>286</v>
+      </c>
+      <c r="H37" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" s="2">
+        <f>AVERAGE(B2:B37)</f>
+        <v>173.61111111111111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="2">
+        <v>173.61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <v>254</v>
+      </c>
+      <c r="C2" s="2">
+        <v>236</v>
+      </c>
+      <c r="D2">
+        <v>173.71</v>
+      </c>
+      <c r="E2">
+        <v>141.85</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2">
+        <v>236</v>
+      </c>
+      <c r="J2">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>162</v>
+      </c>
+      <c r="C3" s="2">
+        <v>138</v>
+      </c>
+      <c r="D3">
+        <v>173.71</v>
+      </c>
+      <c r="E3">
+        <v>141.85</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>138</v>
+      </c>
+      <c r="J3">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>181</v>
+      </c>
+      <c r="C4" s="2">
+        <v>135</v>
+      </c>
+      <c r="D4">
+        <v>173.71</v>
+      </c>
+      <c r="E4">
+        <v>141.85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>135</v>
+      </c>
+      <c r="J4">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>141</v>
+      </c>
+      <c r="C5" s="2">
+        <v>107</v>
+      </c>
+      <c r="D5">
+        <v>173.71</v>
+      </c>
+      <c r="E5">
+        <v>141.85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>107</v>
+      </c>
+      <c r="J5">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>203</v>
+      </c>
+      <c r="C6" s="2">
+        <v>137</v>
+      </c>
+      <c r="D6">
+        <v>173.71</v>
+      </c>
+      <c r="E6">
+        <v>141.85</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>137</v>
+      </c>
+      <c r="J6">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>169</v>
+      </c>
+      <c r="C7" s="2">
+        <v>132</v>
+      </c>
+      <c r="D7">
+        <v>173.71</v>
+      </c>
+      <c r="E7">
+        <v>141.85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>132</v>
+      </c>
+      <c r="J7">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>179</v>
+      </c>
+      <c r="C8" s="2">
+        <v>142</v>
+      </c>
+      <c r="D8">
+        <v>173.71</v>
+      </c>
+      <c r="E8">
+        <v>141.85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2">
+        <v>142</v>
+      </c>
+      <c r="J8">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>139</v>
+      </c>
+      <c r="C9" s="2">
+        <v>95</v>
+      </c>
+      <c r="D9">
+        <v>173.71</v>
+      </c>
+      <c r="E9">
+        <v>141.85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <v>95</v>
+      </c>
+      <c r="J9">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>150</v>
+      </c>
+      <c r="C10" s="2">
+        <v>134</v>
+      </c>
+      <c r="D10">
+        <v>173.71</v>
+      </c>
+      <c r="E10">
+        <v>141.85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2">
+        <v>134</v>
+      </c>
+      <c r="J10">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>134</v>
+      </c>
+      <c r="C11" s="2">
+        <v>134</v>
+      </c>
+      <c r="D11">
+        <v>173.71</v>
+      </c>
+      <c r="E11">
+        <v>141.85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="2">
+        <v>134</v>
+      </c>
+      <c r="J11">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>200</v>
+      </c>
+      <c r="C12" s="2">
+        <v>168</v>
+      </c>
+      <c r="D12">
+        <v>173.71</v>
+      </c>
+      <c r="E12">
+        <v>141.85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="2">
+        <v>168</v>
+      </c>
+      <c r="J12">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>130</v>
+      </c>
+      <c r="C13" s="2">
+        <v>87</v>
+      </c>
+      <c r="D13">
+        <v>173.71</v>
+      </c>
+      <c r="E13">
+        <v>141.85</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="2">
+        <v>87</v>
+      </c>
+      <c r="J13">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>175</v>
+      </c>
+      <c r="C14" s="2">
+        <v>142</v>
+      </c>
+      <c r="D14">
+        <v>173.71</v>
+      </c>
+      <c r="E14">
+        <v>141.85</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2">
+        <v>142</v>
+      </c>
+      <c r="J14">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>216</v>
+      </c>
+      <c r="C15" s="2">
+        <v>182</v>
+      </c>
+      <c r="D15">
+        <v>173.71</v>
+      </c>
+      <c r="E15">
+        <v>141.85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2">
+        <v>182</v>
+      </c>
+      <c r="J15">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>146</v>
+      </c>
+      <c r="C16" s="2">
+        <v>118</v>
+      </c>
+      <c r="D16">
+        <v>173.71</v>
+      </c>
+      <c r="E16">
+        <v>141.85</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2">
+        <v>118</v>
+      </c>
+      <c r="J16">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>162</v>
+      </c>
+      <c r="C17" s="2">
+        <v>110</v>
+      </c>
+      <c r="D17">
+        <v>173.71</v>
+      </c>
+      <c r="E17">
+        <v>141.85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="2">
+        <v>110</v>
+      </c>
+      <c r="J17">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>165</v>
+      </c>
+      <c r="C18" s="2">
+        <v>149</v>
+      </c>
+      <c r="D18">
+        <v>173.71</v>
+      </c>
+      <c r="E18">
+        <v>141.85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="2">
+        <v>149</v>
+      </c>
+      <c r="J18">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>186</v>
+      </c>
+      <c r="C19" s="2">
+        <v>123</v>
+      </c>
+      <c r="D19">
+        <v>173.71</v>
+      </c>
+      <c r="E19">
+        <v>141.85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="2">
+        <v>123</v>
+      </c>
+      <c r="J19">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>185</v>
+      </c>
+      <c r="C20" s="2">
+        <v>142</v>
+      </c>
+      <c r="D20">
+        <v>173.71</v>
+      </c>
+      <c r="E20">
+        <v>141.85</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2">
+        <v>142</v>
+      </c>
+      <c r="J20">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>159</v>
+      </c>
+      <c r="C21" s="2">
+        <v>122</v>
+      </c>
+      <c r="D21">
+        <v>173.71</v>
+      </c>
+      <c r="E21">
+        <v>141.85</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="2">
+        <v>122</v>
+      </c>
+      <c r="J21">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>186</v>
+      </c>
+      <c r="C22" s="2">
+        <v>157</v>
+      </c>
+      <c r="D22">
+        <v>173.71</v>
+      </c>
+      <c r="E22">
+        <v>141.85</v>
+      </c>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="2">
+        <v>157</v>
+      </c>
+      <c r="J22">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>219</v>
+      </c>
+      <c r="C23" s="2">
+        <v>186</v>
+      </c>
+      <c r="D23">
+        <v>173.71</v>
+      </c>
+      <c r="E23">
+        <v>141.85</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="2">
+        <v>186</v>
+      </c>
+      <c r="J23">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>143</v>
+      </c>
+      <c r="C24" s="2">
+        <v>120</v>
+      </c>
+      <c r="D24">
+        <v>173.71</v>
+      </c>
+      <c r="E24">
+        <v>141.85</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="2">
+        <v>120</v>
+      </c>
+      <c r="J24">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2">
+        <v>177</v>
+      </c>
+      <c r="C25" s="2">
+        <v>131</v>
+      </c>
+      <c r="D25">
+        <v>173.71</v>
+      </c>
+      <c r="E25">
+        <v>141.85</v>
+      </c>
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="2">
+        <v>131</v>
+      </c>
+      <c r="J25">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>114</v>
+      </c>
+      <c r="C26" s="2">
+        <v>105</v>
+      </c>
+      <c r="D26">
+        <v>173.71</v>
+      </c>
+      <c r="E26">
+        <v>141.85</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="2">
+        <v>105</v>
+      </c>
+      <c r="J26">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>151</v>
+      </c>
+      <c r="C27" s="2">
+        <v>125</v>
+      </c>
+      <c r="D27">
+        <v>173.71</v>
+      </c>
+      <c r="E27">
+        <v>141.85</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="2">
+        <v>125</v>
+      </c>
+      <c r="J27">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>176</v>
+      </c>
+      <c r="C28" s="2">
+        <v>146</v>
+      </c>
+      <c r="D28">
+        <v>173.71</v>
+      </c>
+      <c r="E28">
+        <v>141.85</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="2">
+        <v>146</v>
+      </c>
+      <c r="J28">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>196</v>
+      </c>
+      <c r="C29" s="2">
+        <v>169</v>
+      </c>
+      <c r="D29">
+        <v>173.71</v>
+      </c>
+      <c r="E29">
+        <v>141.85</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="2">
+        <v>169</v>
+      </c>
+      <c r="J29">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>139</v>
+      </c>
+      <c r="C30" s="2">
+        <v>139</v>
+      </c>
+      <c r="D30">
+        <v>173.71</v>
+      </c>
+      <c r="E30">
+        <v>141.85</v>
+      </c>
+      <c r="H30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="2">
+        <v>139</v>
+      </c>
+      <c r="J30">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>153</v>
+      </c>
+      <c r="C31" s="2">
+        <v>116</v>
+      </c>
+      <c r="D31">
+        <v>173.71</v>
+      </c>
+      <c r="E31">
+        <v>141.85</v>
+      </c>
+      <c r="H31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="2">
+        <v>116</v>
+      </c>
+      <c r="J31">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
+        <v>156</v>
+      </c>
+      <c r="C32" s="2">
+        <v>118</v>
+      </c>
+      <c r="D32">
+        <v>173.71</v>
+      </c>
+      <c r="E32">
+        <v>141.85</v>
+      </c>
+      <c r="H32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="2">
+        <v>118</v>
+      </c>
+      <c r="J32">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2">
+        <v>189</v>
+      </c>
+      <c r="C33" s="2">
+        <v>150</v>
+      </c>
+      <c r="D33">
+        <v>173.71</v>
+      </c>
+      <c r="E33">
+        <v>141.85</v>
+      </c>
+      <c r="H33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="2">
+        <v>150</v>
+      </c>
+      <c r="J33">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2">
+        <v>185</v>
+      </c>
+      <c r="C34" s="2">
+        <v>169</v>
+      </c>
+      <c r="D34">
+        <v>173.71</v>
+      </c>
+      <c r="E34">
+        <v>141.85</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="2">
+        <v>169</v>
+      </c>
+      <c r="J34">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2">
+        <v>286</v>
+      </c>
+      <c r="C35" s="2">
+        <v>259</v>
+      </c>
+      <c r="D35">
+        <v>173.71</v>
+      </c>
+      <c r="E35">
+        <v>141.85</v>
+      </c>
+      <c r="H35" t="s">
+        <v>36</v>
+      </c>
+      <c r="I35" s="2">
+        <v>259</v>
+      </c>
+      <c r="J35">
+        <v>141.85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removing some people's homework from the data files.
</commit_message>
<xml_diff>
--- a/Assignments/ChartBuilder/Exercise1/Chartbuilder1.xlsx
+++ b/Assignments/ChartBuilder/Exercise1/Chartbuilder1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30000" yWindow="285" windowWidth="21720" windowHeight="13620" tabRatio="500"/>
+    <workbookView xWindow="8660" yWindow="2100" windowWidth="21720" windowHeight="13620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="States' Plans" sheetId="4" r:id="rId4"/>
     <sheet name="Bronze v Catastrophic" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -196,12 +196,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,25 +727,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1955,18 +1955,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2388,17 +2388,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2644,21 +2644,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3525,21 +3530,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4458,5 +4468,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>